<commit_message>
Izmir ogrenci yurtlari - Selenium
</commit_message>
<xml_diff>
--- a/izmir_yurtlar_DF.xlsx
+++ b/izmir_yurtlar_DF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\coding\yurtlar_proje\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D8346B-A17D-455E-91EC-23AEA6C1065F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50B4F61-83A5-48C5-8205-5FB6F85AB709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3252,8 +3252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:L1"/>
+    <sheetView tabSelected="1" topLeftCell="A156" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>